<commit_message>
calculate distance between to point and save it as an excel file
</commit_message>
<xml_diff>
--- a/haversine_distant/lanetest5.xlsx
+++ b/haversine_distant/lanetest5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsls\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjswl\python__\python_practice\haversine_distant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589C161D-DB0C-4436-80F5-7E1392CCB65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C3943-796F-4F72-9424-805CE7AC04E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lanetest5" sheetId="1" r:id="rId1"/>
@@ -993,18 +993,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G334"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" customWidth="1"/>
-    <col min="4" max="5" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="5" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>36.635266659999999</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>36.635275</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>127.31848960000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>36.63528333</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>127.3184792</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>36.635291670000001</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>127.31846880000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>36.635300000000001</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>127.3184584</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>36.635308330000001</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>127.318448</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>36.635316670000002</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>127.3184376</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>36.635317710000002</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>127.3184272</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>36.635318750000003</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>127.3184167</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>36.635319789999997</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>127.31840630000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>36.635320829999998</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>127.3183959</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>36.635321879999999</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>127.31838550000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>36.63532292</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>127.318375</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>36.635323960000001</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>127.3183646</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>36.635325000000002</v>
       </c>
@@ -1234,12 +1234,12 @@
         <v>127.3183542</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>36.635326050000003</v>
       </c>
       <c r="B17">
-        <v>1273182396</v>
+        <v>127.3182396</v>
       </c>
       <c r="D17">
         <v>36.635381250000002</v>
@@ -1248,7 +1248,7 @@
         <v>127.31834379999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>36.635327089999997</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>127.31833330000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>36.635328129999998</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>127.31833330000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>36.635329169999999</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>127.31833330000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>36.635330209999999</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>127.31833330000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>36.63533125</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>127.31833330000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>36.635332290000001</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>127.3183229</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>36.635333340000003</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>127.3183125</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>36.635341670000003</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>127.3183021</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>36.635350000000003</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>127.3182917</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>36.635358330000003</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>127.3182813</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>36.635366670000003</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>127.3182709</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>36.635367709999997</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>127.31826049999999</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>36.635368749999998</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>127.31825000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36.635369789999999</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>127.3182396</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>36.635370829999999</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>127.3182292</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>36.635371880000001</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>127.3182188</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>36.635372920000002</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>127.31820829999999</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36.635373960000003</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>127.3181979</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36.635375000000003</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>127.31818749999999</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36.635376049999998</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>127.3181771</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36.635377089999999</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>127.31816670000001</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36.635378129999999</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>127.31816000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>36.63537917</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>127.31815330000001</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>36.635380210000001</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>127.31813990000001</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>36.635381250000002</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>127.31813099999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>36.635382290000003</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>127.3181191</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>36.635383330000003</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>127.3181123</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>36.635391669999997</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>127.3181045</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>36.635399999999997</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>127.31809560000001</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>36.635408329999997</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>127.3180854</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>36.635416669999998</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>127.31807379999999</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>36.635417709999999</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>127.3180606</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>36.635418749999999</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>127.3180535</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>36.63541979</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>127.318046</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>36.635420830000001</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>127.31803789999999</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>36.635421880000003</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>127.31802930000001</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>36.635422920000003</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>127.31802020000001</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>36.635423959999997</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>127.31801040000001</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>36.635424999999998</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>127.318</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>36.63542605</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>127.318</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>36.63542709</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>127.318</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>36.635428130000001</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>127.318</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>36.635429170000002</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>127.318</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>36.635430210000003</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>127.3179892</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>36.635431250000003</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>127.3179785</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>36.635432289999997</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>127.3179713</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>36.635433329999998</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>127.3179617</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>36.635441669999999</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>127.317949</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>36.635449999999999</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>127.31794170000001</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>36.63545834</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>127.3179334</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>36.63546667</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>127.3179239</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>36.635475</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>127.317913</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>36.63548333</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>127.31790049999999</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>36.635484380000001</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>127.3178939</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>36.635485420000002</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>127.3178868</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>36.635486460000003</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>127.3178793</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>36.635487500000004</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>127.31787129999999</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>36.635488549999998</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>127.31786270000001</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>36.635489589999999</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>127.3178535</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>36.63549063</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>127.3178437</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>36.63549167</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>127.3178333</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>36.635492720000002</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>127.3178333</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>36.635493760000003</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>127.3178333</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>36.635494799999996</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>127.31782320000001</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>36.635495839999997</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>127.3178132</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>36.635496879999998</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>127.31780639999999</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>36.635497919999999</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>127.3177975</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>36.63549896</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>127.3177855</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>36.6355</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>127.31777870000001</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>36.63550833</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>127.3177709</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>36.635516670000001</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>127.31776189999999</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>36.635525000000001</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>127.3177517</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>36.635533330000001</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>127.31774009999999</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>36.635541670000002</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>127.31773389999999</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>36.635550000000002</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>127.31772719999999</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>36.635554169999999</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>127.3177202</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>36.635558330000002</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>127.31771259999999</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>36.635562489999998</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>127.3177046</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>36.635566650000001</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>127.317696</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>36.635570819999998</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>127.3176868</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>36.635574980000001</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>127.3176771</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>36.635579139999997</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>127.3176667</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>36.6355833</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>127.31765590000001</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>36.635581219999999</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>127.31764509999999</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>36.635579139999997</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>127.317638</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>36.635577060000003</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>127.3176284</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>36.635574980000001</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>127.3176157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>36.6355729</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>127.3176084</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>36.635570819999998</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>127.3176</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>36.635568739999997</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>127.31759049999999</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>36.635566670000003</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>127.3175796</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>36.635575000000003</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>127.3175672</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>36.635583330000003</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>127.31756059999999</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>36.635591669999997</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>127.3175535</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>36.635599999999997</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>127.31754599999999</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>36.635601049999998</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>127.3175379</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>36.635602089999999</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>127.3175293</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>36.63560313</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>127.3175202</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>36.635604170000001</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>127.3175104</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>36.635605210000001</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>127.3175</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>36.635606250000002</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>127.3175</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>36.635607290000003</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>127.3175</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>36.635608329999997</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>127.3175</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>36.635609379999998</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>127.3175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>36.635610419999999</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>127.3174899</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>36.63561146</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>127.3174798</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>36.635612500000001</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>127.3174731</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>36.635613540000001</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>127.3174641</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>36.635614580000002</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>127.31745220000001</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>36.635615620000003</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>127.3174453</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>36.635616669999997</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>127.3174375</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>36.635624999999997</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>127.3174286</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>36.635633329999997</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>127.31741839999999</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>36.635641669999998</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>127.3174068</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>36.635649999999998</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>127.31740050000001</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>36.635658329999998</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>127.3173939</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>36.635666669999999</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>127.31738679999999</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>36.635668750000001</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>127.3173793</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>36.635670830000002</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>127.3173713</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>36.635672919999998</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>127.3173627</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>36.635674999999999</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>127.3173535</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>36.635677090000001</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>127.3173437</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>36.635679170000003</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>36.635681249999998</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>36.635683329999999</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>36.635685420000001</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>36.635687500000003</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>36.635689589999998</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>36.63569167</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>36.635693760000002</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>127.3173333</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>36.635695839999997</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>127.3173232</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>36.635697919999998</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>127.3173132</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>36.6357</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>127.31730640000001</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>36.63570833</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>127.3172975</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>36.635716670000001</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>127.3172855</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>36.635717710000002</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>127.3172787</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>36.635718750000002</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>127.3172709</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>36.635719790000003</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>127.31726190000001</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>36.635720829999997</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>127.3172517</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>36.635721879999998</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>127.31724010000001</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>36.635722919999999</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>127.31723390000001</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>36.63572396</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>127.3172272</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>36.635725000000001</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>127.31722019999999</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>36.635726050000002</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>127.3172126</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>36.635727090000003</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>127.3172046</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>36.635728129999997</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>127.317196</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>36.635729169999998</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>127.3171868</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>36.635730209999998</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>127.31717709999999</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>36.635731249999999</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>127.3171667</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>36.63573229</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>127.3171562</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>36.635733330000001</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>127.31714580000001</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>36.635741670000002</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>127.3171354</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>36.635750000000002</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>127.317125</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>36.6357833</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>127.3171146</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>36.635766670000002</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>127.3171042</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>36.635767710000003</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>127.31709379999999</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>36.635768749999997</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>127.31708329999999</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>36.635769789999998</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>127.3170729</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>36.635770829999998</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>127.31706250000001</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>36.63577188</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>127.3170521</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>36.635772920000001</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>127.3170417</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>36.635773960000002</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>127.3170313</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>36.635775000000002</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>127.3170209</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>36.635776049999997</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>127.31701049999999</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>36.635777089999998</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>127.31699999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>36.635778129999998</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>127.31699999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>36.635779169999999</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>127.31699999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>36.63578021</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>127.31699999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>36.635781250000001</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>127.31699999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>36.635782290000002</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>127.3169896</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>36.635783330000002</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>127.31697920000001</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>36.635791670000003</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>127.3169688</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>36.635800000000003</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>127.3169584</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>36.635808330000003</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>127.316948</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>36.635816669999997</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>127.3169376</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>36.635824999999997</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>127.31692719999999</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>36.635833329999997</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>127.31691669999999</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>36.635834379999999</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>127.3169063</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>36.635835419999999</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>127.31689590000001</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>36.63583646</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>127.3168855</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>36.635837500000001</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>127.316875</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>36.635838550000003</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>127.3168646</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>36.635839590000003</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>127.31685419999999</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>36.635840629999997</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>127.3168438</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>36.635841669999998</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>127.3168333</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>36.635842719999999</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>127.3168333</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>36.63584376</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>127.3168333</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>36.635844800000001</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>127.3168333</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>36.635845840000002</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>127.3168333</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>36.635846880000003</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>127.31682290000001</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>36.635847920000003</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>127.3168125</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>36.635848959999997</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>127.3168021</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>36.635849999999998</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>127.3167917</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>36.635858329999998</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>127.3167813</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>36.635866669999999</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>127.31677089999999</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>36.63586875</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>127.3167605</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>36.635870830000002</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>127.31675</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>36.635872919999997</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>127.31673960000001</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>36.635874999999999</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>127.3167292</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>36.635877090000001</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>127.3167188</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>36.635879170000003</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>127.3167083</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>36.635881249999997</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>127.31669789999999</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>36.635883329999999</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>127.3166875</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>36.635885420000001</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>127.31667710000001</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>36.635887500000003</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>127.3166667</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>36.635889589999998</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>127.3166562</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>36.635891669999999</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>127.3166458</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>36.635893760000002</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>127.3166354</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>36.635895840000003</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>127.316625</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>36.635897919999998</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>127.31661459999999</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>36.635899999999999</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>127.3166042</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>36.635908329999999</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>127.31659380000001</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>36.63591667</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>127.3165833</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>36.635925</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>127.3165729</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>36.63593333</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>127.3165625</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>36.635941670000001</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>127.3165521</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>36.635950000000001</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>127.3165417</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>36.635951050000003</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>127.31653129999999</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>36.635952090000004</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>127.3165209</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>36.635953129999997</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>127.31651050000001</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>36.635954169999998</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>127.3165</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>36.635955209999999</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>127.3165</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>36.63595625</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>127.3165</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>36.63595729</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>127.3165</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>36.635958330000001</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>127.3165</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>36.635959380000003</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>127.3164896</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>36.635960420000004</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>127.3164792</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>36.635961459999997</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>127.3164688</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>36.635962499999998</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>127.3164584</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>36.635963539999999</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>127.31644799999999</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>36.63596458</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>127.3164376</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>36.63596562</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>127.31642720000001</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>36.635966670000002</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>127.3164167</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>36.635975000000002</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>127.3164063</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>36.635983330000002</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>127.3163959</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>36.635991670000003</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>127.3163855</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>36.636000000000003</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>127.31637499999999</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>36.660083299999997</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>127.3163646</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>36.636016669999997</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>127.31635420000001</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>36.636018749999998</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>127.3163438</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>36.63602083</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>36.636022920000002</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>36.636024999999997</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>36.636027089999999</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>36.63602917</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>36.636031250000002</v>
       </c>
@@ -4692,7 +4692,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>36.636033329999997</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>36.636035419999999</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>36.6360375</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>127.3163333</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>36.636039590000003</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>127.3163229</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>36.636041669999997</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>127.3163125</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>36.63604376</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>127.3163021</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>36.636045840000001</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>127.31629169999999</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>36.636047920000003</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>127.3162813</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>36.636049999999997</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>127.31627090000001</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>36.636058329999997</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>127.3162605</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>36.636066669999998</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>127.31625</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>36.636074999999998</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>127.3162396</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>36.636083329999998</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>127.3162292</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>36.636091669999999</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>127.3162188</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>36.636099999999999</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>127.3162083</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>36.636101050000001</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>127.31619790000001</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>36.636102090000001</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>127.3161875</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>36.636103130000002</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>127.3161771</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>36.636104170000003</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>127.3161667</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>36.636105209999997</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>127.31615619999999</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>36.636106249999997</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>127.3161458</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>36.636107289999998</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>127.31613539999999</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>36.636108329999999</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>127.316125</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>36.636109380000001</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>127.31611460000001</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>36.636110420000001</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>127.3161042</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>36.636111460000002</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>127.3160938</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>36.636112500000003</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>127.3160833</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>36.636113539999997</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>127.31607289999999</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>36.636114579999997</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>127.3160625</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>36.636115619999998</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>127.31605209999999</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>36.63611667</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>127.3160417</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>36.636125</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>127.31603130000001</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>36.63613333</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>127.3160209</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>36.636135420000002</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>127.3160105</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>36.636137499999997</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>127.316</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>36.636139589999999</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>127.316</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>36.636141670000001</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>127.316</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>36.636143760000003</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>127.316</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>36.636145839999998</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>127.316</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>36.636147919999999</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>127.31598959999999</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>36.636150000000001</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>127.3159792</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>36.636152090000003</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>127.31596879999999</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>36.636154169999998</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>127.3159584</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>36.636156249999999</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>127.31594800000001</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>36.636158330000001</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>127.3159376</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>36.636160420000003</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>127.3159272</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>36.636162499999998</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>127.3159167</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>36.636164579999999</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>127.31590629999999</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>36.636166670000001</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>127.3158959</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>36.636175000000001</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>127.31588549999999</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>36.636183330000001</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>127.31587500000001</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>36.636191670000002</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>127.3158646</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>36.636200000000002</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>127.3158542</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>36.636202089999998</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>127.3158438</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>36.636204169999999</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>127.31583329999999</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>36.636206250000001</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>127.3158229</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>36.636208330000002</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>127.31581250000001</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>36.636208330000002</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>127.3158021</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>36.636208330000002</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>127.31579170000001</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>36.636208330000002</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>127.3157813</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>36.636208330000002</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>127.3157709</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>36.636209379999997</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>127.3157605</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>36.636210419999998</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>127.31574999999999</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>36.636211459999998</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>127.3157396</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>36.636212499999999</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>127.31572920000001</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>36.63621354</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>127.3157188</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>36.636214580000001</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>127.3157083</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>36.636215620000002</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>127.3156979</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>36.636216670000003</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>127.3156875</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>36.636225000000003</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>127.3156771</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>36.636233330000003</v>
       </c>

</xml_diff>